<commit_message>
project updated location manage
</commit_message>
<xml_diff>
--- a/SevenrmartSupermarket/src/main/java/Resources/ProjectTestdata.xlsx
+++ b/SevenrmartSupermarket/src/main/java/Resources/ProjectTestdata.xlsx
@@ -8,21 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PROJECTS\eclipse-workspace\SevenrmartSupermarket\src\main\java\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2531F698-4E3A-4FD4-AAFC-A65AB20B88D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF611DF-D6F3-4667-87B0-13658E368B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3552" yWindow="1680" windowWidth="17280" windowHeight="8964" firstSheet="6" activeTab="9" xr2:uid="{AF1BC2BB-CBA9-4CC0-AF8C-1DE4E652C66E}"/>
+    <workbookView xWindow="4248" yWindow="2376" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{AF1BC2BB-CBA9-4CC0-AF8C-1DE4E652C66E}"/>
   </bookViews>
   <sheets>
-    <sheet name="LogInDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
+    <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
+    <sheet name="PushNotification" sheetId="8" r:id="rId2"/>
     <sheet name="SiteName" sheetId="9" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="10" r:id="rId4"/>
+    <sheet name="SelectCategory" sheetId="10" r:id="rId4"/>
     <sheet name="ManageLocation" sheetId="5" r:id="rId5"/>
     <sheet name="SearchLocationWithName" sheetId="6" r:id="rId6"/>
     <sheet name="ManageSlider" sheetId="7" r:id="rId7"/>
-    <sheet name="InvalidDetails" sheetId="2" r:id="rId8"/>
-    <sheet name="InvalidPassword" sheetId="3" r:id="rId9"/>
-    <sheet name="LogOutVerify" sheetId="4" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,20 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t>addmin</t>
-  </si>
-  <si>
-    <t>https://groceryapp.uniqassosiates.com/admin/login</t>
-  </si>
-  <si>
-    <t>ADMMin</t>
-  </si>
-  <si>
     <t>https://groceryapp.uniqassosiates.com/admin/list-location</t>
   </si>
   <si>
@@ -61,13 +49,43 @@
   </si>
   <si>
     <t>https://groceryapp.uniqassosiates.com/admin/home</t>
+  </si>
+  <si>
+    <t>https://groceryapp.uniqassosiates.com/admin</t>
+  </si>
+  <si>
+    <t>Manage Location</t>
+  </si>
+  <si>
+    <t>Push Notifications</t>
+  </si>
+  <si>
+    <t>twenty</t>
+  </si>
+  <si>
+    <t>Wales</t>
+  </si>
+  <si>
+    <t>Manage Slider</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>mega offer</t>
+  </si>
+  <si>
+    <t>New Church Street</t>
+  </si>
+  <si>
+    <t>garden street</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +97,18 @@
       <sz val="7"/>
       <color rgb="FF202124"/>
       <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
       <family val="3"/>
     </font>
   </fonts>
@@ -102,9 +132,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46FFF8D3-57B6-463F-90D3-8FEEAC4CB4E5}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,43 +474,39 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7104C35-6404-413D-B012-0A4E26B700C7}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BADA4E9-97AF-48CD-A5DC-73DF09224AF1}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="44.109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BADA4E9-97AF-48CD-A5DC-73DF09224AF1}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -492,7 +524,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -503,36 +535,78 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342AF692-D251-4E2F-8F3A-2833CEFA1B6B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A63A5D-3BC0-45B1-9B37-CDE6D2D0D779}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A63A5D-3BC0-45B1-9B37-CDE6D2D0D779}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="63.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -548,7 +622,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -558,79 +632,28 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AF3FDF-DBA9-4244-9D2E-C7C2F9883399}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709AF2DD-B451-4C96-B278-8AC9667E69E6}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="44.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD458F6-016D-4188-A6C8-2DA0FE60E880}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="44.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>